<commit_message>
ACE-179: changed Integral rule chinese
</commit_message>
<xml_diff>
--- a/Assets/Resources/Language/Language.xlsx
+++ b/Assets/Resources/Language/Language.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Jawad Ahmad\01 Unity Projects\ACE\Assets\Resources\Language\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ACC5E9-0982-48F2-9E3B-A090051C1A40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73749244-947C-40C3-AAEA-5A7BEE1A8665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8100" yWindow="1605" windowWidth="17025" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,9 +1455,6 @@
     <t>INTEGRAL RULE</t>
   </si>
   <si>
-    <t>积分规则</t>
-  </si>
-  <si>
     <t>Don't Have An Account?</t>
   </si>
   <si>
@@ -1468,6 +1465,9 @@
   </si>
   <si>
     <t>&lt;color=#79E84B&gt;&lt;link=Sign Up Here!&gt;&lt;u&gt;在此註冊！&lt;/u&gt;&lt;/link&gt;&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>積分規則</t>
   </si>
 </sst>
 </file>
@@ -1960,8 +1960,8 @@
   </sheetPr>
   <dimension ref="A1:Z1050"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="C114" sqref="C114"/>
+    <sheetView tabSelected="1" topLeftCell="A244" workbookViewId="0">
+      <selection activeCell="C255" sqref="C255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5738,13 +5738,13 @@
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B113" s="27" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C113" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D113" s="27"/>
       <c r="E113" s="27"/>
@@ -5772,13 +5772,13 @@
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
@@ -10422,7 +10422,7 @@
         <v>449</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="D255" s="1"/>
       <c r="E255" s="1"/>

</xml_diff>